<commit_message>
Implementacion mongodb falta correcta autenticación
</commit_message>
<xml_diff>
--- a/src/main/java/es/uniovi/asw/agentes.xlsx
+++ b/src/main/java/es/uniovi/asw/agentes.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,18 +39,12 @@
     <t>Juan</t>
   </si>
   <si>
-    <t>45,032N65,366W</t>
-  </si>
-  <si>
     <t>administrador@gmail.com</t>
   </si>
   <si>
     <t>#456123</t>
   </si>
   <si>
-    <t>31,032N65,366W</t>
-  </si>
-  <si>
     <t>administrador2@gmail.com</t>
   </si>
   <si>
@@ -79,12 +73,18 @@
   </si>
   <si>
     <t>entidad2@gmail.com</t>
+  </si>
+  <si>
+    <t>45,032N65,06W</t>
+  </si>
+  <si>
+    <t>31,032N56,43W</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -407,19 +407,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,90 +435,94 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" t="s">
         <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
       </c>
       <c r="E3" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
       </c>
       <c r="E4" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E5" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E6" s="2">
         <v>3</v>
       </c>
     </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7"/>
+      <c r="F7" s="2"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1" xr:uid="{5521E897-6F31-4716-80D1-9D0509952A34}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{DE5AC212-95EE-4810-B605-EA5419752B21}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{2BC84A10-B0BB-462C-9DC6-B2BABDA20DE1}"/>
-    <hyperlink ref="C2" r:id="rId4" xr:uid="{8841ADE8-C2A3-47F6-A23B-A1CC6B5F95A7}"/>
-    <hyperlink ref="C5" r:id="rId5" xr:uid="{B087F94B-AA59-4EC1-8E4C-C24A920B308E}"/>
-    <hyperlink ref="C6" r:id="rId6" xr:uid="{F01F437B-05DA-4B54-9459-B2B583732DAF}"/>
+    <hyperlink ref="C1" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId4"/>
+    <hyperlink ref="C5" r:id="rId5"/>
+    <hyperlink ref="C6" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>

</xml_diff>